<commit_message>
update the part of code
</commit_message>
<xml_diff>
--- a/Vtiger.WCSM23.AutomationFramework/src/test/resources/TestData.xlsx
+++ b/Vtiger.WCSM23.AutomationFramework/src/test/resources/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pakki\git\repository\Vtiger.WCSM23.AutomationFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76AA8C76-3992-47CE-B00B-9DBE91FEA789}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{203A62F0-1F21-4DD0-B610-72B27CE432B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="3360" windowWidth="17280" windowHeight="8880" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Organization" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="51">
   <si>
     <t>Test_case</t>
   </si>
@@ -156,12 +156,6 @@
     <t>Retail</t>
   </si>
   <si>
-    <t>studentName</t>
-  </si>
-  <si>
-    <t>Reddy</t>
-  </si>
-  <si>
     <t>Enter Task Name</t>
   </si>
   <si>
@@ -187,9 +181,6 @@
   </si>
   <si>
     <t>Complete test cases and execute in postman</t>
-  </si>
-  <si>
-    <t>Marks</t>
   </si>
 </sst>
 </file>
@@ -803,10 +794,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F37F200-48C7-443E-A646-0DE0722F0E3E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,35 +807,23 @@
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>32</v>
       </c>
       <c r="B2" t="s">
         <v>33</v>
       </c>
-      <c r="C2" t="s">
-        <v>43</v>
-      </c>
-      <c r="D2">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>34</v>
       </c>
@@ -852,7 +831,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -860,7 +839,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>38</v>
       </c>
@@ -868,7 +847,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>40</v>
       </c>
@@ -898,46 +877,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B2">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B3">
         <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B4">
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>